<commit_message>
Change user's realname to non-blank
</commit_message>
<xml_diff>
--- a/media/xlsx/detail/TEA-A6I-75.xlsx
+++ b/media/xlsx/detail/TEA-A6I-75.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="73">
   <si>
     <t>设备品质异常停机单</t>
   </si>
@@ -73,6 +73,9 @@
     <t>停机原因</t>
   </si>
   <si>
+    <t>1234123412341234123412341234123412341234123412341234123412341234123412341234123412341234123412341234</t>
+  </si>
+  <si>
     <t>通知生产人员</t>
   </si>
   <si>
@@ -88,6 +91,9 @@
     <t>受害起止时间</t>
   </si>
   <si>
+    <t>2018/10/17 09:23:00-2018/10/17 09:23:00</t>
+  </si>
+  <si>
     <t>调查报告</t>
   </si>
   <si>
@@ -127,30 +133,27 @@
     <t>责任工程签字</t>
   </si>
   <si>
+    <t>00002</t>
+  </si>
+  <si>
     <t>生产领班签核</t>
   </si>
   <si>
     <t>工程签字时间</t>
   </si>
   <si>
-    <t>2018/10/16 08:58:19</t>
+    <t>2018/10/16 08:58:00</t>
   </si>
   <si>
     <t>生产签字时间</t>
   </si>
   <si>
-    <t>2018/10/16 08:57:54</t>
-  </si>
-  <si>
     <t>设备品质异常复机单 2，id：54</t>
   </si>
   <si>
     <t>申请复机人员</t>
   </si>
   <si>
-    <t>00002</t>
-  </si>
-  <si>
     <t>申请时间</t>
   </si>
   <si>
@@ -217,7 +220,10 @@
     <t>11</t>
   </si>
   <si>
-    <t>2018/10/16 09:15:39</t>
+    <t>2018/10/16 09:51:00</t>
+  </si>
+  <si>
+    <t>3333</t>
   </si>
   <si>
     <t>生产批注</t>
@@ -226,7 +232,7 @@
     <t>最新批注</t>
   </si>
   <si>
-    <t>admin/邓肯的: 1</t>
+    <t>admin/邓肯: 1</t>
   </si>
 </sst>
 </file>
@@ -266,12 +272,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -280,14 +301,16 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -591,158 +614,183 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
     </row>
     <row r="3" spans="2:7">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="2:7">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" t="s">
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="2:7">
-      <c r="B8" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7">
-      <c r="B9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7">
-      <c r="B10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7">
-      <c r="B11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="2"/>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" t="s">
-        <v>29</v>
-      </c>
+      <c r="B12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -751,106 +799,132 @@
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="2:7">
-      <c r="B14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="B14" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="C14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="2"/>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7">
-      <c r="B16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7">
-      <c r="B17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7">
-      <c r="B18" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="2:7">
-      <c r="B19" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7">
-      <c r="B20" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7">
-      <c r="B21" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7">
-      <c r="B22" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" t="s">
-        <v>32</v>
-      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
     </row>
     <row r="23" spans="2:7">
       <c r="B23" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -859,19 +933,22 @@
       <c r="G23" s="4"/>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" s="2"/>
     </row>
     <row r="25" spans="2:7">
       <c r="B25" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -880,95 +957,116 @@
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="B26" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E26" t="s">
+      <c r="C26" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="D26" s="2"/>
+      <c r="E26" s="2" t="s">
         <v>60</v>
       </c>
+      <c r="F26" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G26" s="2"/>
     </row>
     <row r="27" spans="2:7">
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="B28" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="2:7">
+      <c r="B29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="B30" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="2:7">
+      <c r="B31" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C27" t="s">
-        <v>62</v>
-      </c>
-      <c r="E27" t="s">
-        <v>63</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7">
-      <c r="B28" s="1" t="s">
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="2:7">
+      <c r="B32" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="2:7">
+      <c r="B33" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C28" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7">
-      <c r="B29" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="2:7">
-      <c r="B30" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30" t="s">
-        <v>45</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7">
-      <c r="B31" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7">
-      <c r="B32" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7">
-      <c r="B33" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C33" t="s">
-        <v>29</v>
-      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
     </row>
     <row r="34" spans="2:7">
       <c r="B34" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -977,28 +1075,28 @@
       <c r="G34" s="4"/>
     </row>
     <row r="35" spans="2:7">
-      <c r="B35" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C35" t="s">
-        <v>66</v>
-      </c>
-      <c r="D35" s="1" t="s">
+      <c r="B35" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E35" t="s">
-        <v>66</v>
-      </c>
-      <c r="F35" s="1" t="s">
+      <c r="C35" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G35" t="s">
-        <v>66</v>
+      <c r="E35" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="2:7">
       <c r="B36" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -1007,58 +1105,69 @@
       <c r="G36" s="3"/>
     </row>
     <row r="37" spans="2:7">
-      <c r="B37" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C37" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" t="s">
-        <v>59</v>
-      </c>
+      <c r="B37" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
     </row>
     <row r="38" spans="2:7">
-      <c r="B38" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C38" t="s">
-        <v>67</v>
-      </c>
-      <c r="E38" t="s">
-        <v>63</v>
+      <c r="B38" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="2:7">
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C39" t="s">
-        <v>29</v>
-      </c>
-      <c r="E39" t="s">
-        <v>34</v>
-      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G39" s="2"/>
     </row>
     <row r="40" spans="2:7">
-      <c r="B40" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
+      <c r="B40" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
     </row>
     <row r="41" spans="2:7">
-      <c r="B41" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C41" t="s">
-        <v>70</v>
-      </c>
+      <c r="B41" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="44">
+  <mergeCells count="45">
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="B8:G8"/>
@@ -1068,6 +1177,7 @@
     <mergeCell ref="C12:G12"/>
     <mergeCell ref="B13:G13"/>
     <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:G14"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="C16:D16"/>

</xml_diff>